<commit_message>
change condition files + add stimuli
</commit_message>
<xml_diff>
--- a/orange_green_purple/condition_file_orange_green_purple.xlsx
+++ b/orange_green_purple/condition_file_orange_green_purple.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rochellekaper/Desktop/Both_Tasks/orange_green_purple/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E7C2502-950D-2A42-9D5F-DF60FD012527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EEDF191-6EFA-ED46-A3FE-AE22FEE08CF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29380" windowHeight="18380" xr2:uid="{DA1428FE-1F6B-D84E-A641-D81E17FE7399}"/>
   </bookViews>
@@ -4821,8 +4821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29A4020E-9A69-1D46-A565-9220EE152F5E}">
   <dimension ref="A1:M301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B294" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E301"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -4977,7 +4977,7 @@
         <v>108</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F4" s="2">
         <v>-0.25</v>
@@ -5018,7 +5018,7 @@
         <v>110</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F5" s="2">
         <v>-0.25</v>
@@ -5264,7 +5264,7 @@
         <v>139</v>
       </c>
       <c r="E11" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F11" s="2">
         <v>-0.25</v>
@@ -5279,7 +5279,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>30</v>
+        <v>120</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>15</v>

</xml_diff>